<commit_message>
Add file upload support with logging and API integration
Co-authored-by: ha01iujie6 <ha01iujie6@gmail.com>
</commit_message>
<xml_diff>
--- a/logs/training_records.xlsx
+++ b/logs/training_records.xlsx
@@ -12,6 +12,8 @@
     <sheet name="forms" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="completions" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="closures" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="uploads" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="operations" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -417,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,6 +490,28 @@
       <c r="D3" t="inlineStr">
         <is>
           <t>E999</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:45:15.474683</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:45:15.474654</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>a8c1ea65-a4e7-456d-b788-2d96dc55cb51</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>E777</t>
         </is>
       </c>
     </row>
@@ -935,4 +959,269 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>write_time</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>session_id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>employee_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>step_number</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>field_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>original_filename</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>saved_path</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>file_size_bytes</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>mime_type</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:45:15.535796</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:45:15.535782</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>a8c1ea65-a4e7-456d-b788-2d96dc55cb51</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>E777</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>file_hukou</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>hukou.png</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>logs/uploads/E777/a8c1ea65-a4e7-456d-b788-2d96dc55cb51/20250813T144515_hukou.png</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>image/png</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>write_time</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>session_id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>employee_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>operation_type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>step_number</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>extra</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:45:15.503579</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:45:15.474654</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>a8c1ea65-a4e7-456d-b788-2d96dc55cb51</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>E777</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>start</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>start</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:45:15.562053</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-08-13T14:45:15.535782</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>a8c1ea65-a4e7-456d-b788-2d96dc55cb51</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>E777</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>upload</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>file_hukou</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>hukou.png</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>logs/uploads/E777/a8c1ea65-a4e7-456d-b788-2d96dc55cb51/20250813T144515_hukou.png</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>